<commit_message>
Mise à jour du suivi de projet
</commit_message>
<xml_diff>
--- a/suivi_projet.xlsx
+++ b/suivi_projet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfelixlasalle-my.sharepoint.com/personal/david_louboutin_stfelixlasalle_fr/Documents/Stage_Missions/Mission n°1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\stage\Stage_2025_ST_felixDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{75EA9391-73D1-4593-9065-3A32AC43A01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90E4D620-D7AA-41FA-9606-408E485CAD3E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696125A9-07EE-4697-B81F-F993577B7D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{701D3BB8-75BD-43D3-8126-0FBE5F0BB179}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Lecture de la documentation de l'afficheur à LED défilant Mc Crypt n°590996</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Création d'un dépôt GIT depuis GitHub</t>
+  </si>
+  <si>
+    <t>Lecture de la documentation de l'adaptateur RS232 à RJ45 "CSE-H53N" par Sollae</t>
+  </si>
+  <si>
+    <t>CSE-H53N | RS-232 Serial To Ethernet Converter</t>
   </si>
 </sst>
 </file>
@@ -469,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4521D194-E84C-4CFA-9C75-1EDA66349D08}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>45803</v>
       </c>
@@ -498,7 +504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -507,7 +513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -517,139 +523,141 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>45804</v>
+      <c r="A5" s="8"/>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <v>45805</v>
+        <v>45804</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <v>45806</v>
+        <v>45805</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <v>45807</v>
+        <v>45806</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
-        <v>45808</v>
+        <v>45807</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <v>45809</v>
+        <v>45808</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
-        <v>45810</v>
+        <v>45809</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>45811</v>
+        <v>45810</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>45812</v>
+        <v>45811</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>45813</v>
+        <v>45812</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>45814</v>
+        <v>45813</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>45815</v>
+        <v>45814</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>45816</v>
+        <v>45815</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>45817</v>
+        <v>45816</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>45818</v>
+        <v>45817</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>45819</v>
+        <v>45818</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>45820</v>
+        <v>45819</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>45821</v>
+        <v>45820</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>45822</v>
+        <v>45821</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>45823</v>
+        <v>45822</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>45824</v>
+        <v>45823</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>45825</v>
+        <v>45824</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>45826</v>
+        <v>45825</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <v>45827</v>
+        <v>45826</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
+        <v>45827</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
         <v>45828</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://www.manualslib.fr/manual/127901/Mc-Crypt-59-09-96.html" xr:uid="{263E46E5-5A86-4CAB-9BE0-696E9371DDC1}"/>
-    <hyperlink ref="C4" r:id="rId2" display="http://tvaira.free.fr/projets/docs/panneau-mc-crypte-590996.pdf" xr:uid="{255C19F3-5FD2-41AB-B059-5949C05ED287}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>